<commit_message>
feat : add auto eval
</commit_message>
<xml_diff>
--- a/Auto-Eval-ASI1-r1.xlsx
+++ b/Auto-Eval-ASI1-r1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7CED5ED-F300-43B1-80A3-718265E1ABB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917BA0B7-A98E-4BF0-BA41-A04C10606A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auto-Evaluation" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Auteur</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -97,7 +97,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Auteur</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
@@ -885,15 +885,15 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="32" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D1" s="19" t="s">
         <v>59</v>
       </c>
@@ -925,7 +925,7 @@
       <c r="T1" s="20"/>
       <c r="U1" s="20"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
@@ -981,7 +981,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -1001,7 +1001,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
         <v>47</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>0</v>
       </c>
@@ -1086,7 +1086,7 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="9"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="22" t="s">
         <v>4</v>
@@ -1108,7 +1108,7 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="9"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
@@ -1117,8 +1117,8 @@
       <c r="D7" t="s">
         <v>48</v>
       </c>
-      <c r="E7" t="s">
-        <v>53</v>
+      <c r="E7" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="F7" t="s">
         <v>53</v>
@@ -1160,7 +1160,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
@@ -1169,8 +1169,8 @@
       <c r="D8" t="s">
         <v>48</v>
       </c>
-      <c r="E8" t="s">
-        <v>53</v>
+      <c r="E8" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="F8" t="s">
         <v>53</v>
@@ -1212,7 +1212,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
@@ -1221,8 +1221,8 @@
       <c r="D9" t="s">
         <v>48</v>
       </c>
-      <c r="E9" t="s">
-        <v>53</v>
+      <c r="E9" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="F9" t="s">
         <v>53</v>
@@ -1264,7 +1264,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
@@ -1273,8 +1273,8 @@
       <c r="D10" t="s">
         <v>49</v>
       </c>
-      <c r="E10" t="s">
-        <v>53</v>
+      <c r="E10" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="F10" t="s">
         <v>53</v>
@@ -1316,7 +1316,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
@@ -1325,8 +1325,8 @@
       <c r="D11" t="s">
         <v>48</v>
       </c>
-      <c r="E11" t="s">
-        <v>53</v>
+      <c r="E11" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="F11" t="s">
         <v>53</v>
@@ -1368,7 +1368,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
@@ -1377,8 +1377,8 @@
       <c r="D12" t="s">
         <v>53</v>
       </c>
-      <c r="E12" t="s">
-        <v>53</v>
+      <c r="E12" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="F12" t="s">
         <v>53</v>
@@ -1420,7 +1420,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4" t="s">
@@ -1429,8 +1429,8 @@
       <c r="D13" t="s">
         <v>53</v>
       </c>
-      <c r="E13" t="s">
-        <v>53</v>
+      <c r="E13" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="F13" t="s">
         <v>53</v>
@@ -1472,7 +1472,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4" t="s">
@@ -1524,7 +1524,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4" t="s">
@@ -1576,7 +1576,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4" t="s">
@@ -1628,7 +1628,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
@@ -1680,7 +1680,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4" t="s">
@@ -1732,7 +1732,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4" t="s">
@@ -1742,7 +1742,7 @@
         <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F19" t="s">
         <v>53</v>
@@ -1784,7 +1784,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
@@ -1794,7 +1794,7 @@
         <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s">
         <v>53</v>
@@ -1836,7 +1836,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4" t="s">
@@ -1846,7 +1846,7 @@
         <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
         <v>53</v>
@@ -1888,7 +1888,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
@@ -1898,7 +1898,7 @@
         <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s">
         <v>53</v>
@@ -1940,7 +1940,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
@@ -1950,7 +1950,7 @@
         <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F23" t="s">
         <v>53</v>
@@ -1992,7 +1992,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4" t="s">
@@ -2002,7 +2002,7 @@
         <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F24" t="s">
         <v>53</v>
@@ -2044,7 +2044,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4" t="s">
@@ -2054,7 +2054,7 @@
         <v>53</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F25" t="s">
         <v>53</v>
@@ -2096,7 +2096,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4" t="s">
@@ -2106,7 +2106,7 @@
         <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F26" t="s">
         <v>53</v>
@@ -2148,7 +2148,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4" t="s">
@@ -2200,7 +2200,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4" t="s">
@@ -2252,7 +2252,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4" t="s">
@@ -2262,7 +2262,7 @@
         <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F29" t="s">
         <v>53</v>
@@ -2304,7 +2304,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="4" t="s">
@@ -2314,7 +2314,7 @@
         <v>53</v>
       </c>
       <c r="E30" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F30" t="s">
         <v>53</v>
@@ -2356,7 +2356,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="4" t="s">
@@ -2408,7 +2408,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4" t="s">
@@ -2460,7 +2460,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4" t="s">
@@ -2512,7 +2512,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4" t="s">
@@ -2564,7 +2564,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4" t="s">
@@ -2574,7 +2574,7 @@
         <v>53</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F35" t="s">
         <v>53</v>
@@ -2616,7 +2616,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="22" t="s">
         <v>15</v>
@@ -2638,7 +2638,7 @@
       <c r="Q36" s="3"/>
       <c r="R36" s="9"/>
     </row>
-    <row r="37" spans="1:18" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4" t="s">
@@ -2648,7 +2648,7 @@
         <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F37" t="s">
         <v>53</v>
@@ -2690,7 +2690,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4" t="s">
@@ -2700,7 +2700,7 @@
         <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F38" t="s">
         <v>53</v>
@@ -2742,7 +2742,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4" t="s">
@@ -2794,7 +2794,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4" t="s">
@@ -2846,7 +2846,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
@@ -2856,7 +2856,7 @@
         <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F41" t="s">
         <v>53</v>
@@ -2898,7 +2898,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="4" t="s">
@@ -2908,7 +2908,7 @@
         <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F42" t="s">
         <v>53</v>
@@ -2950,7 +2950,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="4" t="s">
@@ -2960,7 +2960,7 @@
         <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F43" t="s">
         <v>53</v>
@@ -3002,7 +3002,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="4" t="s">
@@ -3012,7 +3012,7 @@
         <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F44" t="s">
         <v>53</v>
@@ -3054,7 +3054,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="4" t="s">
@@ -3064,7 +3064,7 @@
         <v>53</v>
       </c>
       <c r="E45" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F45" t="s">
         <v>53</v>
@@ -3106,7 +3106,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
@@ -3116,7 +3116,7 @@
         <v>53</v>
       </c>
       <c r="E46" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F46" t="s">
         <v>53</v>
@@ -3158,7 +3158,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="4" t="s">
@@ -3168,7 +3168,7 @@
         <v>53</v>
       </c>
       <c r="E47" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F47" t="s">
         <v>53</v>
@@ -3210,7 +3210,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
@@ -3220,7 +3220,7 @@
         <v>53</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F48" t="s">
         <v>53</v>
@@ -3262,7 +3262,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="4" t="s">
@@ -3314,7 +3314,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4" t="s">
@@ -3366,7 +3366,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4" t="s">
@@ -3418,7 +3418,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="4" t="s">
@@ -3470,7 +3470,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="4" t="s">
@@ -3522,7 +3522,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="25.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="4" t="s">
@@ -3574,7 +3574,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="S1:U1"/>
@@ -3655,34 +3655,34 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>

</xml_diff>